<commit_message>
Updated the details from the URS doc
Updated the details from the URS doc
</commit_message>
<xml_diff>
--- a/TECH/ANALYSIS/RTM/Requirement traceability matrix.xlsx
+++ b/TECH/ANALYSIS/RTM/Requirement traceability matrix.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmb/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED05A10-ED8A-074E-9856-88E5DA34C14D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14280" xr2:uid="{433097B7-DA32-6A44-9BD9-0BDF32C4284D}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28590" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
     <sheet name="References" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>Use cases</t>
   </si>
@@ -39,9 +33,6 @@
     <t>Test cases</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Close error report</t>
   </si>
   <si>
@@ -166,12 +157,93 @@
   </si>
   <si>
     <t>URS</t>
+  </si>
+  <si>
+    <t>3.2.3.1</t>
+  </si>
+  <si>
+    <t>3.2.3.4</t>
+  </si>
+  <si>
+    <t>3.2.3.3</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>3.2.3.6</t>
+  </si>
+  <si>
+    <t>3.2.5.2</t>
+  </si>
+  <si>
+    <t>3.2.6</t>
+  </si>
+  <si>
+    <t>3.2.7</t>
+  </si>
+  <si>
+    <t>Auditing &amp; Traceability</t>
+  </si>
+  <si>
+    <t>3.2.9</t>
+  </si>
+  <si>
+    <t>3.2.8</t>
+  </si>
+  <si>
+    <t>System Alert and Notifications</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Real time dashboard</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Data Download</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Station Management</t>
+  </si>
+  <si>
+    <t>User Login and Access Control</t>
+  </si>
+  <si>
+    <t>Sl No</t>
+  </si>
+  <si>
+    <t>3.2.2.2</t>
+  </si>
+  <si>
+    <t>User/Access Control Mapping</t>
+  </si>
+  <si>
+    <t>3.2.3.5</t>
+  </si>
+  <si>
+    <t>User/Station Mapping</t>
+  </si>
+  <si>
+    <t>3.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -248,14 +320,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,359 +634,600 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BC7C38-14AD-7849-9771-05C5D513A675}">
-  <dimension ref="A1:J21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C2" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3">
+      <c r="G7">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="1">
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1">
         <v>3.3</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6">
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="E21" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="E22" t="s">
         <v>6</v>
       </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10">
+      <c r="G22">
         <v>21</v>
       </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
         <v>17</v>
       </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="1" t="s">
+      <c r="G23">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
-      </c>
-      <c r="G15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="1" t="s">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <v>12</v>
-      </c>
-      <c r="G19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>39</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L23">
+    <sortCondition ref="B2:B23"/>
+    <sortCondition ref="C2:C23"/>
+  </sortState>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D9:D18 D2:D7 D8 D20 D21:D22 D23" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{111CA8D2-888C-164F-98BA-83D0A96E81C2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>References!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G21</xm:sqref>
+          <xm:sqref>H25 H2:H22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{811C5531-1200-8E4E-9E62-A2825EE95A4C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>References!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I21</xm:sqref>
+          <xm:sqref>J25 J2:J22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -923,54 +1236,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898F662B-580E-CE42-9B96-FE6FA1CAFB66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the RTM with Req
Updated the RTM with Requirements
</commit_message>
<xml_diff>
--- a/TECH/ANALYSIS/RTM/Requirement traceability matrix.xlsx
+++ b/TECH/ANALYSIS/RTM/Requirement traceability matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28590" windowHeight="12495"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="23256" windowHeight="12492"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>Use cases</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>3.2</t>
+  </si>
+  <si>
+    <t>3.2.5.1</t>
+  </si>
+  <si>
+    <t>Data Capture</t>
+  </si>
+  <si>
+    <t>3.2.5</t>
+  </si>
+  <si>
+    <t>Central Data Maagement</t>
   </si>
 </sst>
 </file>
@@ -645,23 +657,23 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="10" width="16.875" customWidth="1"/>
+    <col min="9" max="9" width="19.09765625" customWidth="1"/>
+    <col min="10" max="10" width="16.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>65</v>
       </c>
@@ -692,7 +704,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -715,7 +727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -738,7 +750,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -761,7 +773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -784,7 +796,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -807,7 +819,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -830,7 +842,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -853,7 +865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -876,7 +888,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -899,7 +911,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -922,7 +934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -945,7 +957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -968,7 +980,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -991,196 +1003,214 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G15">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>72</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.8</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.9</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3.6</v>
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3.3</v>
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="D21" s="1">
-        <v>3.8</v>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G21">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
       <c r="D22" s="1">
-        <v>3.9</v>
+        <v>3.6</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>31</v>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.3</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1191,12 +1221,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1212,7 +1242,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D9:D18 D2:D7 D8 D20 D21:D22 D23" numberStoredAsText="1"/>
+    <ignoredError sqref="D18:D21 D23 D2:D14" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1221,13 +1251,13 @@
           <x14:formula1>
             <xm:f>References!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H25 H2:H22</xm:sqref>
+          <xm:sqref>H25 H2:H14 H16:H23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>References!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J25 J2:J22</xm:sqref>
+          <xm:sqref>J25 J2:J14 J16:J23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1243,13 +1273,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1257,7 +1287,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1265,7 +1295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1273,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1311,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>

</xml_diff>